<commit_message>
Implemented MTDf - testing now
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank\Dropbox\Private\Projekte\_GITHUB\FrankyUCIChessEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA49D18-9D5A-4783-A26C-57B0D9F5AD4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8C4630-FB4B-4D5A-848F-CC20851F2B86}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7697" yWindow="3967" windowWidth="31641" windowHeight="21535" activeTab="3" xr2:uid="{3AD9B36B-4EE6-004A-91F3-199B9971943E}"/>
+    <workbookView xWindow="7697" yWindow="3967" windowWidth="31641" windowHeight="21535" activeTab="4" xr2:uid="{3AD9B36B-4EE6-004A-91F3-199B9971943E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
     <sheet name="Tabelle4" sheetId="4" r:id="rId4"/>
+    <sheet name="Tabelle5" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$B$2406</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8604" uniqueCount="1684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8641" uniqueCount="1697">
   <si>
     <t>R6R/3Q4/1Q4Q1/4Q3/2Q4Q/Q4Q2/pp1Q4/kBNN1KB1 w - - 0 1</t>
   </si>
@@ -5089,6 +5090,45 @@
   </si>
   <si>
     <t>e 02</t>
+  </si>
+  <si>
+    <t>----------------------------------------------------------------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Name    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Move </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Nodes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Nps </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Time </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> e2e4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASPIRATION   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTDf         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> d2b2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> e2a6 </t>
   </si>
 </sst>
 </file>
@@ -5136,11 +5176,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -64619,8 +64662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C80DC72-1792-4098-AFB7-32B3678DBBA0}">
   <dimension ref="A2:J2399"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -83489,4 +83532,286 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31113DE1-C6B8-4936-8EF3-926E01D12D37}">
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1686</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1688</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1684</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>1566</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C3" s="1">
+        <v>53300</v>
+      </c>
+      <c r="D3" s="1">
+        <v>200375</v>
+      </c>
+      <c r="E3">
+        <v>265</v>
+      </c>
+      <c r="F3" t="s">
+        <v>403</v>
+      </c>
+      <c r="M3" t="str">
+        <f>A3</f>
+        <v xml:space="preserve">ALL          </v>
+      </c>
+      <c r="N3" s="2">
+        <f>SUMIF($A:$A,$A3,C:C)</f>
+        <v>185207</v>
+      </c>
+      <c r="O3" s="2">
+        <f t="shared" ref="O3:P5" si="0">SUMIF($A:$A,$A3,D:D)</f>
+        <v>1865615</v>
+      </c>
+      <c r="P3" s="2">
+        <f t="shared" si="0"/>
+        <v>639</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C4" s="1">
+        <v>69659</v>
+      </c>
+      <c r="D4" s="1">
+        <v>295165</v>
+      </c>
+      <c r="E4">
+        <v>235</v>
+      </c>
+      <c r="F4" t="s">
+        <v>403</v>
+      </c>
+      <c r="M4" t="str">
+        <f>A4</f>
+        <v xml:space="preserve">ASPIRATION   </v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N5" si="1">SUMIF($A:$A,$A4,C:C)</f>
+        <v>222790</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" si="0"/>
+        <v>2000436</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" si="0"/>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C5" s="1">
+        <v>32956</v>
+      </c>
+      <c r="D5" s="1">
+        <v>190497</v>
+      </c>
+      <c r="E5">
+        <v>172</v>
+      </c>
+      <c r="F5" t="s">
+        <v>403</v>
+      </c>
+      <c r="M5" t="str">
+        <f>A5</f>
+        <v xml:space="preserve">MTDf         </v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="1"/>
+        <v>380413</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="0"/>
+        <v>962635</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="0"/>
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1317</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1317000</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1317</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1317000</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C9">
+        <v>446</v>
+      </c>
+      <c r="D9" s="1">
+        <v>446000</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1696</v>
+      </c>
+      <c r="C11" s="1">
+        <v>130590</v>
+      </c>
+      <c r="D11" s="1">
+        <v>348240</v>
+      </c>
+      <c r="E11">
+        <v>374</v>
+      </c>
+      <c r="F11" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1696</v>
+      </c>
+      <c r="C12" s="1">
+        <v>151814</v>
+      </c>
+      <c r="D12" s="1">
+        <v>388271</v>
+      </c>
+      <c r="E12">
+        <v>390</v>
+      </c>
+      <c r="F12" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1696</v>
+      </c>
+      <c r="C13" s="1">
+        <v>347011</v>
+      </c>
+      <c r="D13" s="1">
+        <v>326138</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1063</v>
+      </c>
+      <c r="F13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>